<commit_message>
Added new dumpState function to the Arduino
</commit_message>
<xml_diff>
--- a/doc/systems/Arduino REST.xlsx
+++ b/doc/systems/Arduino REST.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5376" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5376"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="156">
   <si>
     <t>Variable Name</t>
   </si>
@@ -502,6 +502,12 @@
   </si>
   <si>
     <t>number of milliseconds since last heartbeat</t>
+  </si>
+  <si>
+    <t>dumpState</t>
+  </si>
+  <si>
+    <t>Returns a JSON object containing the entire state</t>
   </si>
 </sst>
 </file>
@@ -863,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5245,10 +5251,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA20"/>
+  <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5618,6 +5624,23 @@
         <v>120</v>
       </c>
     </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished writing the parse/pack routines
</commit_message>
<xml_diff>
--- a/doc/systems/Arduino REST.xlsx
+++ b/doc/systems/Arduino REST.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5376"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5376" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Functions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -869,7 +869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -5253,7 +5253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated Arduino REST to include break up of dumpState function
</commit_message>
<xml_diff>
--- a/doc/systems/Arduino REST.xlsx
+++ b/doc/systems/Arduino REST.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="164">
   <si>
     <t>Variable Name</t>
   </si>
@@ -504,10 +504,34 @@
     <t>number of milliseconds since last heartbeat</t>
   </si>
   <si>
-    <t>dumpState</t>
-  </si>
-  <si>
-    <t>Returns a JSON object containing the entire state</t>
+    <t>dumpCoreState</t>
+  </si>
+  <si>
+    <t>dumpOrientationState</t>
+  </si>
+  <si>
+    <t>dumpInputState</t>
+  </si>
+  <si>
+    <t>dumpRawInputState</t>
+  </si>
+  <si>
+    <t>dumpOutputState</t>
+  </si>
+  <si>
+    <t>Returns a JSON object containing the core state</t>
+  </si>
+  <si>
+    <t>Returns a JSON object containing the input state</t>
+  </si>
+  <si>
+    <t>Returns a JSON object containing the output state</t>
+  </si>
+  <si>
+    <t>Returns a JSON object containing the orientation</t>
+  </si>
+  <si>
+    <t>Returns a JSON object containing the raw input state</t>
   </si>
 </sst>
 </file>
@@ -5251,10 +5275,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA21"/>
+  <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5264,7 +5288,7 @@
     <col min="3" max="3" width="18.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.44140625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5638,7 +5662,75 @@
         <v>120</v>
       </c>
       <c r="F21" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>155</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>